<commit_message>
27.8 - пункты 1-11 ОК (toExel)
</commit_message>
<xml_diff>
--- a/src/main/resources/statistics.xlsx
+++ b/src/main/resources/statistics.xlsx
@@ -12,7 +12,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="6">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="13">
   <si>
     <t>Профиль обучения</t>
   </si>
@@ -26,10 +26,38 @@
     <t>Количество университетов по профилю</t>
   </si>
   <si>
-    <t>Название университета</t>
-  </si>
-  <si>
-    <t>Казанский придуманный Университет</t>
+    <t>Название университетов</t>
+  </si>
+  <si>
+    <t>PHYSICS</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> МВУ
+ МПИ
+</t>
+  </si>
+  <si>
+    <t>MEDICINE</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> МГМУ
+ ТУМ
+ СМИ
+</t>
+  </si>
+  <si>
+    <t>LINGUISTICS</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> ВЛПУ
+</t>
+  </si>
+  <si>
+    <t>MATHEMATICS</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> КУВ
+</t>
   </si>
 </sst>
 </file>
@@ -80,7 +108,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <dimension ref="A1:E2"/>
+  <dimension ref="A1:E5"/>
   <sheetViews>
     <sheetView workbookViewId="0" tabSelected="true"/>
   </sheetViews>
@@ -111,20 +139,71 @@
       </c>
     </row>
     <row r="2">
-      <c r="A2" t="n">
-        <v>0.0</v>
+      <c r="A2" t="s">
+        <v>5</v>
       </c>
       <c r="B2" t="n">
-        <v>4.0</v>
+        <v>4.53000020980835</v>
       </c>
       <c r="C2" t="n">
-        <v>33.0</v>
+        <v>8.0</v>
       </c>
       <c r="D2" t="n">
-        <v>55.0</v>
+        <v>2.0</v>
       </c>
       <c r="E2" t="s">
-        <v>5</v>
+        <v>6</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="s">
+        <v>7</v>
+      </c>
+      <c r="B3" t="n">
+        <v>4.329999923706055</v>
+      </c>
+      <c r="C3" t="n">
+        <v>3.0</v>
+      </c>
+      <c r="D3" t="n">
+        <v>3.0</v>
+      </c>
+      <c r="E3" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="s">
+        <v>9</v>
+      </c>
+      <c r="B4" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="C4" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="D4" t="n">
+        <v>1.0</v>
+      </c>
+      <c r="E4" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="s">
+        <v>11</v>
+      </c>
+      <c r="B5" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="C5" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="D5" t="n">
+        <v>1.0</v>
+      </c>
+      <c r="E5" t="s">
+        <v>12</v>
       </c>
     </row>
   </sheetData>

</xml_diff>